<commit_message>
docs: comments on config file
</commit_message>
<xml_diff>
--- a/Documents/specs/GME_Configuration_Parameters.xlsx
+++ b/Documents/specs/GME_Configuration_Parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>ap_ssid_hidden</t>
   </si>
@@ -147,7 +147,53 @@
     <t>pool.ntp.org</t>
   </si>
   <si>
-    <t>0=Enabled  1=Disabled</t>
+    <t>ssid of the AP to which GME should connect</t>
+  </si>
+  <si>
+    <t>psk of the AP to which GME should connect</t>
+  </si>
+  <si>
+    <t>don't know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GME will acquire an IP address from a dhcp server when connected to the AP? 0:no, 1:yes </t>
+  </si>
+  <si>
+    <t>Static IP address of the GME when dhcp is disabled</t>
+  </si>
+  <si>
+    <t>Gateway of the GME when dhcp is disabled</t>
+  </si>
+  <si>
+    <t>Netmask of the GME when dhcp is disabled</t>
+  </si>
+  <si>
+    <t>ssid of the GME</t>
+  </si>
+  <si>
+    <t>psk to access GME as AP</t>
+  </si>
+  <si>
+    <t>DNS</t>
+  </si>
+  <si>
+    <t>APN</t>
+  </si>
+  <si>
+    <t>don't know (do we support different types of encryption?)</t>
+  </si>
+  <si>
+    <t>IP address leased by a dhcp server</t>
+  </si>
+  <si>
+    <t>IP address of the GME working as AP</t>
+  </si>
+  <si>
+    <t>netmask of the GME working as AP</t>
+  </si>
+  <si>
+    <t>secondo me non serve, perché il modulo non avrà un server dhcp a bordo per distribuire indirizzi
+0=Enabled  1=Disabled</t>
   </si>
 </sst>
 </file>
@@ -283,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,6 +366,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -701,6 +750,9 @@
       <c r="B2">
         <v>30</v>
       </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -709,6 +761,9 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -717,6 +772,9 @@
       <c r="B4">
         <v>30</v>
       </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -728,6 +786,9 @@
       <c r="B6">
         <v>6</v>
       </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -736,16 +797,19 @@
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>43</v>
+      <c r="D8" s="20" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -755,6 +819,9 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
@@ -766,11 +833,17 @@
       <c r="B11">
         <v>30</v>
       </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -779,6 +852,9 @@
       <c r="B13">
         <v>30</v>
       </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -787,6 +863,9 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -795,6 +874,9 @@
       <c r="B15">
         <v>4</v>
       </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -803,6 +885,9 @@
       <c r="B16">
         <v>4</v>
       </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -811,6 +896,9 @@
       <c r="B17">
         <v>4</v>
       </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
@@ -822,6 +910,9 @@
       <c r="B19">
         <v>30</v>
       </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
@@ -832,6 +923,9 @@
       </c>
       <c r="B21">
         <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
docs: added some default values
</commit_message>
<xml_diff>
--- a/Documents/specs/GME_Configuration_Parameters.xlsx
+++ b/Documents/specs/GME_Configuration_Parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>ap_ssid_hidden</t>
   </si>
@@ -48,15 +48,6 @@
     <t>ap_pswd</t>
   </si>
   <si>
-    <t>C_CHAR ap_ip</t>
-  </si>
-  <si>
-    <t>C_CHAR ap_netmask</t>
-  </si>
-  <si>
-    <t>C_CHAR ap_dhcp_ip</t>
-  </si>
-  <si>
     <t>C_CHAR sta_ssid</t>
   </si>
   <si>
@@ -66,27 +57,9 @@
     <t>C_CHAR sta_pswd</t>
   </si>
   <si>
-    <t>C_CHAR sta_static_ip</t>
-  </si>
-  <si>
-    <t>C_CHAR sta_netmask</t>
-  </si>
-  <si>
-    <t>C_CHAR sta_gateway_ip</t>
-  </si>
-  <si>
     <t>C_CHAR apn_name</t>
   </si>
   <si>
-    <t>C_CHAR sta_primary_dns</t>
-  </si>
-  <si>
-    <t>C_CHAR sta_secondary_dns</t>
-  </si>
-  <si>
-    <t>C_CHAR ntp_server_URI</t>
-  </si>
-  <si>
     <t>C_URI MQTT_SERVER</t>
   </si>
   <si>
@@ -96,9 +69,6 @@
     <t>C_BYTE RS485_TTL</t>
   </si>
   <si>
-    <t>C_UINT16 baudrate</t>
-  </si>
-  <si>
     <t>C_PASSWORD</t>
   </si>
   <si>
@@ -151,9 +121,6 @@
   </si>
   <si>
     <t>psk of the AP to which GME should connect</t>
-  </si>
-  <si>
-    <t>don't know</t>
   </si>
   <si>
     <t xml:space="preserve">GME will acquire an IP address from a dhcp server when connected to the AP? 0:no, 1:yes </t>
@@ -194,13 +161,67 @@
   <si>
     <t>secondo me non serve, perché il modulo non avrà un server dhcp a bordo per distribuire indirizzi
 0=Enabled  1=Disabled</t>
+  </si>
+  <si>
+    <t>C_URI ntp_server_URI</t>
+  </si>
+  <si>
+    <t>C_UINT32 baudrate</t>
+  </si>
+  <si>
+    <t>C_IPV4 ap_dhcp_ip</t>
+  </si>
+  <si>
+    <t>C_IPV4 ap_ip</t>
+  </si>
+  <si>
+    <t>C_IPV4 ap_netmask</t>
+  </si>
+  <si>
+    <t>C_IPV4 sta_static_ip</t>
+  </si>
+  <si>
+    <t>C_IPV4 sta_netmask</t>
+  </si>
+  <si>
+    <t>C_IPV4 sta_gateway_ip</t>
+  </si>
+  <si>
+    <t>C_IPV4 sta_primary_dns</t>
+  </si>
+  <si>
+    <t>C_IPV4 sta_secondary_dns</t>
+  </si>
+  <si>
+    <t>C_UINT16 LSS</t>
+  </si>
+  <si>
+    <t>C_UINT16 HSS</t>
+  </si>
+  <si>
+    <t>high speed sampling time</t>
+  </si>
+  <si>
+    <t>low speed sampling time</t>
+  </si>
+  <si>
+    <t>select if AP is broadcasting its IP address (0) or not (1)</t>
+  </si>
+  <si>
+    <t>GME_xxxxxx, xxxxxx is the last part of the MAC</t>
+  </si>
+  <si>
+    <t>192.168.100.1</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +248,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -329,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -368,6 +397,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,24 +724,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -718,8 +754,8 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,16 +767,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -750,8 +786,11 @@
       <c r="B2">
         <v>30</v>
       </c>
+      <c r="C2" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -761,8 +800,9 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3" s="23"/>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -772,33 +812,43 @@
       <c r="B4">
         <v>30</v>
       </c>
+      <c r="C4" s="23">
+        <v>12345678</v>
+      </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
+      <c r="C6" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
+      <c r="C7" s="23" t="s">
+        <v>65</v>
+      </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -809,18 +859,18 @@
         <v>1</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -828,35 +878,36 @@
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>30</v>
       </c>
+      <c r="C11" s="22"/>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -864,40 +915,40 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -905,13 +956,13 @@
     </row>
     <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -919,18 +970,18 @@
     </row>
     <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -941,13 +992,13 @@
     </row>
     <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8">
         <v>64</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -966,18 +1017,18 @@
     </row>
     <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B27" s="8">
         <v>64</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B28" s="14">
         <v>2</v>
@@ -988,29 +1039,29 @@
     </row>
     <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B29" s="14">
         <v>34</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B30" s="11">
         <v>32</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B32" s="8">
         <v>1</v>
@@ -1019,12 +1070,12 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B33" s="11">
         <v>2</v>
@@ -1033,13 +1084,41 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>300</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>60</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="5">
         <f>SUM(B2:B39)</f>
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>